<commit_message>
push to make report legible online
copied wrong folder before(?)
</commit_message>
<xml_diff>
--- a/Inst/extdata/factor_recode.xlsx
+++ b/Inst/extdata/factor_recode.xlsx
@@ -1776,9 +1776,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B7851B2-D8BF-4E15-83E2-74AC9A236FE1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC04FD33-E8B5-40AA-B747-36F39B2FC3EF}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0FF1989-859A-4029-97AB-E3ADF38D1443}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{970515D1-4B84-45D4-BE3A-205923B94B41}"/>
 </file>
</xml_diff>